<commit_message>
Enviando arquivo atualizado Metas.xlsx
</commit_message>
<xml_diff>
--- a/CURSO XPERIUM/LINGUAGEM DAX ESSENCIAL/LIVE2/Bases/Metas.xlsx
+++ b/CURSO XPERIUM/LINGUAGEM DAX ESSENCIAL/LIVE2/Bases/Metas.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\OneDrive - Aprenda Power BI\Cursos Online\_Arquivos\TrilhaExpress_v2.0\Modulo 2\BaseDados\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Cristiano\Curso_GitHub\4_PowerBI\CURSO XPERIUM\LINGUAGEM DAX ESSENCIAL\LIVE2\Bases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66DDB622-8BA2-4B90-9811-2B20EF62517A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{CEF1353F-E079-454E-8E2E-7BAF08CE81E8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12300"/>
   </bookViews>
   <sheets>
     <sheet name="Metas" sheetId="3" r:id="rId1"/>
@@ -50,7 +49,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="&quot;R$&quot;#,##0"/>
   </numFmts>
@@ -443,29 +442,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30669D1E-EEC2-44D4-A30D-5F31E69851AF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z17"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="13.44140625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="13.42578125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="25" width="13.44140625" style="1"/>
-    <col min="26" max="26" width="13.44140625" style="6"/>
-    <col min="27" max="16384" width="13.44140625" style="1"/>
+    <col min="1" max="25" width="13.42578125" style="1"/>
+    <col min="26" max="26" width="13.42578125" style="6"/>
+    <col min="27" max="16384" width="13.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -545,7 +546,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="4">
         <v>102</v>
       </c>
@@ -626,7 +627,7 @@
         <v>3033854.4478095141</v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="4">
         <v>125</v>
       </c>
@@ -707,7 +708,7 @@
         <v>2708056.7045584526</v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>144</v>
       </c>
@@ -788,7 +789,7 @@
         <v>2050895.5573728115</v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>194</v>
       </c>
@@ -869,7 +870,7 @@
         <v>427924.39196785609</v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>196</v>
       </c>
@@ -950,7 +951,7 @@
         <v>2037216.8140251595</v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>215</v>
       </c>
@@ -1031,7 +1032,7 @@
         <v>5247942.733420088</v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>265</v>
       </c>
@@ -1112,7 +1113,7 @@
         <v>3830827.7604236021</v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>285</v>
       </c>
@@ -1193,7 +1194,7 @@
         <v>1651439.5048681421</v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>326</v>
       </c>
@@ -1274,7 +1275,7 @@
         <v>881940.53674829227</v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>660</v>
       </c>
@@ -1355,7 +1356,7 @@
         <v>47213.390337970559</v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>669</v>
       </c>
@@ -1436,7 +1437,7 @@
         <v>1914090.3834700666</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>2</v>
       </c>

</xml_diff>